<commit_message>
added 7-10 years stories
</commit_message>
<xml_diff>
--- a/output/summary_all_texts.xlsx
+++ b/output/summary_all_texts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schia\OneDrive - Alma Mater Studiorum Università di Bologna\Desktop\IMT\TESI\linguistic_pipeline_EEG\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/francesca_schiavon10_studio_unibo_it/Documents/Desktop/IMT/TESI/linguistic_pipeline_EEG/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082A6E0F-00E4-43EE-A5BD-688614C3998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{082A6E0F-00E4-43EE-A5BD-688614C3998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99BBAA6C-671C-4F69-8D0B-347AA8E5275B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{6395D661-BD89-49EA-AF66-F4D7978AA4CD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="702">
   <si>
     <t>text_id</t>
   </si>
@@ -1640,6 +1640,504 @@
   </si>
   <si>
     <t>20.15% ± 2.37%</t>
+  </si>
+  <si>
+    <t>01_710</t>
+  </si>
+  <si>
+    <t>423</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>0.466</t>
+  </si>
+  <si>
+    <t>0.385</t>
+  </si>
+  <si>
+    <t>11.23</t>
+  </si>
+  <si>
+    <t>5.63</t>
+  </si>
+  <si>
+    <t>5.73</t>
+  </si>
+  <si>
+    <t>81.1</t>
+  </si>
+  <si>
+    <t>201 (47.5%)</t>
+  </si>
+  <si>
+    <t>220 (52.0%)</t>
+  </si>
+  <si>
+    <t>61 (14.4%)</t>
+  </si>
+  <si>
+    <t>28 (6.6%)</t>
+  </si>
+  <si>
+    <t>83 (19.6%)</t>
+  </si>
+  <si>
+    <t>['il (7.3%)', 'uno (5.2%)', 'essere (5.0%)', 'e (3.5%)', 'di (2.8%)', 'mamma (2.4%)', 'si (2.4%)', 'Giovanni (2.1%)', 'a (1.9%)', 'ma (1.9%)', 'distratto (1.7%)', 'che (1.7%)', 'tutto (1.4%)', 'non (1.4%)', 'cosa (1.2%)', 'suo (1.2%)', 'fare (0.9%)', 'sì (0.9%)', 'così (0.9%)', 'poi (0.9%)']</t>
+  </si>
+  <si>
+    <t>['di il (1.2%)', 'e cosa (0.7%)', 'i bambini (0.7%)', 'bambini sono (0.7%)', 'sono tutti (0.7%)', 'tutti così (0.7%)', 'giovanni ma (0.5%)', 'mamma ciao (0.5%)', 'ciao mamma (0.5%)', 'e per (0.5%)']</t>
+  </si>
+  <si>
+    <t>02_710</t>
+  </si>
+  <si>
+    <t>434</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>0.422</t>
+  </si>
+  <si>
+    <t>15.73</t>
+  </si>
+  <si>
+    <t>5.39</t>
+  </si>
+  <si>
+    <t>11.16</t>
+  </si>
+  <si>
+    <t>66.56</t>
+  </si>
+  <si>
+    <t>204 (47.0%)</t>
+  </si>
+  <si>
+    <t>224 (51.6%)</t>
+  </si>
+  <si>
+    <t>67 (15.4%)</t>
+  </si>
+  <si>
+    <t>23 (5.3%)</t>
+  </si>
+  <si>
+    <t>95 (21.9%)</t>
+  </si>
+  <si>
+    <t>['il (10.6%)', 'uno (3.5%)', 'essere (3.0%)', 'a (3.0%)', 'e (2.5%)', 'di (2.5%)', 'non (2.3%)', 'che (2.3%)', 'guardia (2.3%)', 'per (2.1%)', 'punta (1.8%)', 'Giovannino (1.6%)', 'ma (1.6%)', 'con (1.6%)', 'fare (1.6%)', 'paese (1.4%)', 'senza (1.4%)', 'si (1.2%)', 'avere (1.2%)', 'dire (1.2%)']</t>
+  </si>
+  <si>
+    <t>['la guardia (2.1%)', 'senza punta (1.2%)', 'il paese (0.9%)', 'a la (0.9%)', 'paese senza (0.7%)', 'punta ma (0.7%)', 'che è (0.7%)', 'disse la (0.7%)', 'di i (0.7%)', 'due schiaffi (0.7%)']</t>
+  </si>
+  <si>
+    <t>03_710</t>
+  </si>
+  <si>
+    <t>436</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>0.475</t>
+  </si>
+  <si>
+    <t>0.411</t>
+  </si>
+  <si>
+    <t>17.61</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>17.68</t>
+  </si>
+  <si>
+    <t>61.8</t>
+  </si>
+  <si>
+    <t>214 (49.1%)</t>
+  </si>
+  <si>
+    <t>217 (49.8%)</t>
+  </si>
+  <si>
+    <t>57 (13.1%)</t>
+  </si>
+  <si>
+    <t>18 (4.1%)</t>
+  </si>
+  <si>
+    <t>119 (27.3%)</t>
+  </si>
+  <si>
+    <t>['il (14.7%)', 'di (4.8%)', 'e (4.4%)', 'uno (4.1%)', 'per (2.5%)', 'campana (1.8%)', 'ci (1.8%)', 'da (1.8%)', 'cannone (1.8%)', 'essere (1.6%)', 'che (1.4%)', 'a (1.4%)', 'Stragenerale (1.4%)', 'guerra (1.1%)', 'nemico (1.1%)', 'tutto (1.1%)', 'si (1.1%)', 'Din (1.1%)', 'Don (1.1%)', 'Dan (1.1%)']</t>
+  </si>
+  <si>
+    <t>['le campane (1.6%)', 'lo stragenerale (1.4%)', 'i nemici (0.9%)', 'din don (0.9%)', 'don dan (0.9%)', 'la guerra (0.7%)', 'il fronte (0.7%)', 'per la (0.7%)', 'di il (0.7%)', 'di i (0.7%)']</t>
+  </si>
+  <si>
+    <t>04_710</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>0.553</t>
+  </si>
+  <si>
+    <t>0.452</t>
+  </si>
+  <si>
+    <t>17.79</t>
+  </si>
+  <si>
+    <t>14.39</t>
+  </si>
+  <si>
+    <t>63.7</t>
+  </si>
+  <si>
+    <t>205 (48.5%)</t>
+  </si>
+  <si>
+    <t>218 (51.5%)</t>
+  </si>
+  <si>
+    <t>64 (15.1%)</t>
+  </si>
+  <si>
+    <t>34 (8.0%)</t>
+  </si>
+  <si>
+    <t>85 (20.1%)</t>
+  </si>
+  <si>
+    <t>['il (10.4%)', 'essere (3.8%)', 'uno (3.5%)', 'e (3.1%)', 'a (2.6%)', 'che (2.4%)', 'in (2.1%)', 'si (1.9%)', 'di (1.7%)', 'viola (1.4%)', 'suo (1.4%)', 'per (1.4%)', 'bianco (1.2%)', 'tutto (1.2%)', 'ne (1.2%)', 'come (1.2%)', 'dire (1.2%)', 'avere (1.2%)', 'orso (0.9%)', 'ma (0.9%)']</t>
+  </si>
+  <si>
+    <t>['il polo (0.9%)', 'l orso (0.9%)', 'orso bianco (0.9%)', 'il suo (0.9%)', 'a il (0.7%)', 'tutto il (0.7%)', 'polo nord (0.5%)', 'l aria (0.5%)', 'la viola (0.5%)', 'per tutto (0.5%)']</t>
+  </si>
+  <si>
+    <t>05_710</t>
+  </si>
+  <si>
+    <t>469</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>0.388</t>
+  </si>
+  <si>
+    <t>21.46</t>
+  </si>
+  <si>
+    <t>11.32</t>
+  </si>
+  <si>
+    <t>60.19</t>
+  </si>
+  <si>
+    <t>236 (50.3%)</t>
+  </si>
+  <si>
+    <t>232 (49.5%)</t>
+  </si>
+  <si>
+    <t>65 (13.9%)</t>
+  </si>
+  <si>
+    <t>19 (4.1%)</t>
+  </si>
+  <si>
+    <t>112 (23.9%)</t>
+  </si>
+  <si>
+    <t>['il (11.3%)', 'di (6.2%)', 'e (5.3%)', 'uno (4.1%)', 'suo (3.0%)', 'in (2.3%)', 'essere (2.1%)', 'Giacomo (1.9%)', 'si (1.7%)', 'più (1.7%)', 'per (1.7%)', 'a (1.5%)', 'vedere (1.5%)', 'non (1.5%)', 'pensiero (1.3%)', 'cristallo (1.1%)', 'come (1.1%)', 'ma (1.1%)', 'gente (1.1%)', 'tutto (1.1%)']</t>
+  </si>
+  <si>
+    <t>['di cristallo (1.1%)', 'la gente (1.1%)', 'giacomo di (0.9%)', 'il suo (0.9%)', 'i suoi (0.9%)', 'suoi pensieri (0.9%)', 'la sua (0.9%)', 'a il (0.6%)', 'cristallo e (0.6%)', 'pensieri di (0.6%)']</t>
+  </si>
+  <si>
+    <t>06_710</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>14.31</t>
+  </si>
+  <si>
+    <t>5.54</t>
+  </si>
+  <si>
+    <t>8.31</t>
+  </si>
+  <si>
+    <t>71.49</t>
+  </si>
+  <si>
+    <t>173 (47.4%)</t>
+  </si>
+  <si>
+    <t>176 (48.2%)</t>
+  </si>
+  <si>
+    <t>61 (16.7%)</t>
+  </si>
+  <si>
+    <t>23 (6.3%)</t>
+  </si>
+  <si>
+    <t>65 (17.8%)</t>
+  </si>
+  <si>
+    <t>['il (8.5%)', 'uno (6.3%)', 'essere (4.7%)', 'di (2.7%)', 'e (2.5%)', 'avere (1.9%)', 'ma (1.6%)', 'non (1.6%)', 'che (1.4%)', 'fare (1.4%)', 'per (1.4%)', 'a (1.4%)', 'guardare (1.4%)', 'quattro (1.4%)', 'più (1.1%)', 'se (1.1%)', 'Dieci (1.1%)', 'con (1.1%)', 'suo (1.1%)', 'ne (1.1%)']</t>
+  </si>
+  <si>
+    <t>['ma la (0.8%)', 'promosso più (0.5%)', 'più due (0.5%)', 'povero dieci (0.5%)', 'che ti (0.5%)', 'ma non (0.5%)', 'un disastro (0.5%)', 'la sottrazione (0.5%)', 'la sua (0.5%)', 'perde un (0.5%)']</t>
+  </si>
+  <si>
+    <t>07_710</t>
+  </si>
+  <si>
+    <t>0.407</t>
+  </si>
+  <si>
+    <t>19.16</t>
+  </si>
+  <si>
+    <t>5.22</t>
+  </si>
+  <si>
+    <t>14.42</t>
+  </si>
+  <si>
+    <t>60.61</t>
+  </si>
+  <si>
+    <t>203 (48.0%)</t>
+  </si>
+  <si>
+    <t>213 (50.4%)</t>
+  </si>
+  <si>
+    <t>73 (17.3%)</t>
+  </si>
+  <si>
+    <t>25 (5.9%)</t>
+  </si>
+  <si>
+    <t>94 (22.2%)</t>
+  </si>
+  <si>
+    <t>['il (8.7%)', 'uno (5.2%)', 'di (5.0%)', 'e (4.7%)', 'cane (2.8%)', 'essere (2.6%)', 'a (2.6%)', 'abbaiare (2.4%)', 'fare (2.4%)', 'avere (2.1%)', 'che (1.9%)', 'da (1.4%)', 'si (1.4%)', 'paese (0.9%)', 'novantanove (0.9%)', 'casetta (0.9%)', 'abitante (0.9%)', 'quello (0.9%)', 'diventare (0.9%)', 'parlare (0.9%)']</t>
+  </si>
+  <si>
+    <t>['i cani (1.2%)', 'gli abitanti (0.9%)', 'di i (0.7%)', 'abitanti di (0.7%)', 'c era (0.5%)', 'una volta (0.5%)', 'strano piccolo (0.5%)', 'piccolo paese (0.5%)', 'con un (0.5%)', 'e ne (0.5%)']</t>
+  </si>
+  <si>
+    <t>08_710</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>0.356</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>5.34</t>
+  </si>
+  <si>
+    <t>13.61</t>
+  </si>
+  <si>
+    <t>63.59</t>
+  </si>
+  <si>
+    <t>219 (51.3%)</t>
+  </si>
+  <si>
+    <t>208 (48.7%)</t>
+  </si>
+  <si>
+    <t>62 (14.5%)</t>
+  </si>
+  <si>
+    <t>12 (2.8%)</t>
+  </si>
+  <si>
+    <t>111 (26.0%)</t>
+  </si>
+  <si>
+    <t>['il (14.3%)', 'di (5.9%)', 'fare (3.5%)', 'e (3.5%)', 'Apollonia (3.0%)', 'marmellata (3.0%)', 'uno (2.8%)', 'a (2.3%)', 'essere (1.9%)', 'avere (1.9%)', 'si (1.6%)', 'imperatore (1.6%)', 'non (1.4%)', 'donnina (1.2%)', 'che (1.2%)', 'da (1.2%)', 'mano (1.2%)', 'in (0.9%)', 'quello (0.9%)', 'ricco (0.9%)']</t>
+  </si>
+  <si>
+    <t>['l apollonia (2.3%)', 'la marmellata (1.9%)', 'l imperatore (1.6%)', 'le mani (0.9%)', 'di il (0.7%)', 'me la (0.7%)', 'marmellata di (0.7%)', 'quella donnina (0.7%)', 'mani d (0.7%)', 'd oro (0.7%)']</t>
+  </si>
+  <si>
+    <t>09_710</t>
+  </si>
+  <si>
+    <t>458</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>0.502</t>
+  </si>
+  <si>
+    <t>0.439</t>
+  </si>
+  <si>
+    <t>24.2</t>
+  </si>
+  <si>
+    <t>5.36</t>
+  </si>
+  <si>
+    <t>11.28</t>
+  </si>
+  <si>
+    <t>59.09</t>
+  </si>
+  <si>
+    <t>239 (52.2%)</t>
+  </si>
+  <si>
+    <t>219 (47.8%)</t>
+  </si>
+  <si>
+    <t>64 (14.0%)</t>
+  </si>
+  <si>
+    <t>18 (3.9%)</t>
+  </si>
+  <si>
+    <t>107 (23.4%)</t>
+  </si>
+  <si>
+    <t>['il (13.8%)', 'di (5.7%)', 'e (3.7%)', 'a (3.7%)', 'essere (3.1%)', 'uno (2.6%)', 'in (2.0%)', 'mario (2.0%)', 'si (1.7%)', 'che (1.7%)', 'casa (1.7%)', 'non (1.3%)', 'per (1.3%)', 'suo (1.3%)', 'da (0.9%)', 'morire (0.9%)', 'sentire (0.9%)', 'loro (0.9%)', 'proprio (0.7%)', 'come (0.7%)']</t>
+  </si>
+  <si>
+    <t>['la casa (1.5%)', 'di la (1.3%)', 'a la (0.9%)', 'in il (0.7%)', 'a il (0.7%)', 'i loro (0.7%)', 'la valtellina (0.4%)', 'un giorno (0.4%)', 'di un (0.4%)', 'il suo (0.4%)']</t>
+  </si>
+  <si>
+    <t>10_710</t>
+  </si>
+  <si>
+    <t>477</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>0.444</t>
+  </si>
+  <si>
+    <t>0.361</t>
+  </si>
+  <si>
+    <t>29.0</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>58.48</t>
+  </si>
+  <si>
+    <t>220 (46.1%)</t>
+  </si>
+  <si>
+    <t>250 (52.4%)</t>
+  </si>
+  <si>
+    <t>88 (18.4%)</t>
+  </si>
+  <si>
+    <t>14 (2.9%)</t>
+  </si>
+  <si>
+    <t>121 (25.4%)</t>
+  </si>
+  <si>
+    <t>['il (10.9%)', 'e (5.0%)', 'di (4.8%)', 'oro (2.5%)', 'uno (2.3%)', 'a (2.3%)', 'fare (2.1%)', 'toccare (2.1%)', 'diventare (2.1%)', 're (1.9%)', 'Mida (1.9%)', 'si (1.9%)', 'per (1.9%)', 'tutto (1.5%)', 'sette (1.5%)', 'andare (1.3%)', 'ora (1.3%)', 'essere (1.0%)', 'gli (1.0%)', 'che (1.0%)']</t>
+  </si>
+  <si>
+    <t>['d oro (2.3%)', 'il re (1.9%)', 're mida (1.9%)', 'sette minuti (0.8%)', 'da il (0.6%)', 'la macchina (0.6%)', 'l incantesimo (0.6%)', 'sette ore (0.6%)', 'ore e (0.6%)', 'e sette (0.6%)']</t>
+  </si>
+  <si>
+    <t>433.50 ± 31.31</t>
+  </si>
+  <si>
+    <t>28.30 ± 8.37</t>
+  </si>
+  <si>
+    <t>211.50 ± 15.44</t>
+  </si>
+  <si>
+    <t>0.49 ± 0.04</t>
+  </si>
+  <si>
+    <t>0.41 ± 0.04</t>
+  </si>
+  <si>
+    <t>18.88 ± 5.05</t>
+  </si>
+  <si>
+    <t>5.34 ± 0.15</t>
+  </si>
+  <si>
+    <t>11.88 ± 3.37</t>
+  </si>
+  <si>
+    <t>64.66 ± 6.96</t>
+  </si>
+  <si>
+    <t>48.74% ± 1.97%</t>
+  </si>
+  <si>
+    <t>50.19% ± 1.65%</t>
+  </si>
+  <si>
+    <t>15.28% ± 1.69%</t>
+  </si>
+  <si>
+    <t>4.99% ± 1.71%</t>
+  </si>
+  <si>
+    <t>22.76% ± 3.03%</t>
   </si>
 </sst>
 </file>
@@ -2146,9 +2644,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2630,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB4F147-2834-492D-A5BC-A21A60783755}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3977,7 +4475,642 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>367</v>
@@ -4561,7 +5694,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>154</v>
       </c>

</xml_diff>